<commit_message>
Convert Json server To SQL (login,signup,forgot, 50% admin)
</commit_message>
<xml_diff>
--- a/LaTiPee.xlsx
+++ b/LaTiPee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0392956804\Documents\GitHub\LaTiPee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khai\Documents\GitHub\LaTiPee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1315727E-974A-46C8-A4AF-E1753DFF1593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86EBBE7-F44B-4D67-943D-56D3C74F5797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F2426AB-354F-4FC1-AF11-9F71120D466A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F2426AB-354F-4FC1-AF11-9F71120D466A}"/>
   </bookViews>
   <sheets>
     <sheet name="LaTiPee" sheetId="1" r:id="rId1"/>
@@ -856,23 +856,23 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="109" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -895,7 +895,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -910,7 +910,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -933,7 +933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -956,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -977,7 +977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -998,7 +998,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1101,7 +1101,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1393,7 +1393,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I25" s="1">
         <v>13</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I26" s="1">
         <v>14</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I27" s="1">
         <v>15</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I28" s="1">
         <v>16</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I29" s="1">
         <v>17</v>
       </c>
@@ -1466,21 +1466,21 @@
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="110.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="110.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1500,7 +1500,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1545,13 +1545,13 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>65</v>
@@ -1560,7 +1560,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1596,13 +1596,13 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>70</v>
@@ -1611,7 +1611,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3</v>
       </c>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>5</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>6</v>
       </c>
@@ -1665,13 +1665,13 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>72</v>
@@ -1680,7 +1680,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>2</v>
       </c>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
         <v>92</v>
@@ -1716,7 +1716,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>2</v>
       </c>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -1752,12 +1752,12 @@
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>97</v>
@@ -1766,7 +1766,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3</v>
       </c>

</xml_diff>